<commit_message>
changed rice and rice noodles sound and crisps and khmer cakes name
</commit_message>
<xml_diff>
--- a/app/src/main/assets/foodList/foods_original.xlsx
+++ b/app/src/main/assets/foodList/foods_original.xlsx
@@ -1313,9 +1313,6 @@
     <t>Khmer cakes</t>
   </si>
   <si>
-    <t>នំក្រូច</t>
-  </si>
-  <si>
     <t>coconut_rice_cake.jpg</t>
   </si>
   <si>
@@ -1325,9 +1322,6 @@
     <t>Crisps</t>
   </si>
   <si>
-    <t>នំំកញ្ចប់</t>
-  </si>
-  <si>
     <t>crisps.jpg</t>
   </si>
   <si>
@@ -1698,6 +1692,12 @@
   </si>
   <si>
     <t>salt.m4a</t>
+  </si>
+  <si>
+    <t>នំក្រួក</t>
+  </si>
+  <si>
+    <t>នំស្រួយៗ</t>
   </si>
 </sst>
 </file>
@@ -2110,8 +2110,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2144,19 +2144,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>448</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2176,19 +2176,19 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2205,22 +2205,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2237,27 +2237,27 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>19</v>
@@ -2272,19 +2272,19 @@
         <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2304,19 +2304,19 @@
         <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2336,19 +2336,19 @@
         <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2368,19 +2368,19 @@
         <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2388,95 +2388,95 @@
         <v>424</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>425</v>
+        <v>552</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>427</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>429</v>
+        <v>553</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2487,7 +2487,7 @@
         <v>421</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>422</v>
@@ -2496,147 +2496,147 @@
         <v>423</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="F13" t="s">
+        <v>494</v>
+      </c>
+      <c r="G13" t="s">
+        <v>494</v>
+      </c>
+      <c r="H13" t="s">
+        <v>495</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="F13" t="s">
-        <v>496</v>
-      </c>
-      <c r="G13" t="s">
-        <v>496</v>
-      </c>
-      <c r="H13" t="s">
-        <v>497</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F14" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G14" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H14" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="F15" t="s">
+        <v>495</v>
+      </c>
+      <c r="G15" t="s">
+        <v>494</v>
+      </c>
+      <c r="H15" t="s">
+        <v>494</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="F15" t="s">
-        <v>497</v>
-      </c>
-      <c r="G15" t="s">
-        <v>496</v>
-      </c>
-      <c r="H15" t="s">
-        <v>496</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F16" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G16" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H16" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2656,19 +2656,19 @@
         <v>38</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2688,19 +2688,19 @@
         <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2720,19 +2720,19 @@
         <v>46</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2752,19 +2752,19 @@
         <v>50</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2784,19 +2784,19 @@
         <v>54</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2816,19 +2816,19 @@
         <v>58</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2848,19 +2848,19 @@
         <v>62</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2880,19 +2880,19 @@
         <v>66</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2912,19 +2912,19 @@
         <v>70</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2944,19 +2944,19 @@
         <v>74</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2976,19 +2976,19 @@
         <v>78</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3008,19 +3008,19 @@
         <v>82</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3040,19 +3040,19 @@
         <v>86</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3072,19 +3072,19 @@
         <v>90</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3104,19 +3104,19 @@
         <v>94</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3136,19 +3136,19 @@
         <v>98</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3168,19 +3168,19 @@
         <v>102</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3200,19 +3200,19 @@
         <v>106</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3232,19 +3232,19 @@
         <v>110</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3264,19 +3264,19 @@
         <v>113</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3296,19 +3296,19 @@
         <v>117</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3328,19 +3328,19 @@
         <v>121</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3360,19 +3360,19 @@
         <v>125</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3392,19 +3392,19 @@
         <v>129</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3424,19 +3424,19 @@
         <v>133</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3456,19 +3456,19 @@
         <v>137</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3488,19 +3488,19 @@
         <v>141</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3520,19 +3520,19 @@
         <v>145</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3552,19 +3552,19 @@
         <v>149</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3584,19 +3584,19 @@
         <v>153</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3616,19 +3616,19 @@
         <v>157</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3648,19 +3648,19 @@
         <v>161</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3680,19 +3680,19 @@
         <v>165</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3712,19 +3712,19 @@
         <v>169</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3744,19 +3744,19 @@
         <v>173</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3776,19 +3776,19 @@
         <v>178</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3808,19 +3808,19 @@
         <v>182</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3840,19 +3840,19 @@
         <v>186</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3872,19 +3872,19 @@
         <v>190</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3904,19 +3904,19 @@
         <v>194</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3936,19 +3936,19 @@
         <v>198</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -3968,147 +3968,147 @@
         <v>202</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>176</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>176</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>176</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>176</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4128,19 +4128,19 @@
         <v>223</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4160,19 +4160,19 @@
         <v>227</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4192,19 +4192,19 @@
         <v>231</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4224,19 +4224,19 @@
         <v>235</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4256,19 +4256,19 @@
         <v>239</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4288,51 +4288,51 @@
         <v>242</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>221</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4346,25 +4346,25 @@
         <v>205</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>206</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4378,25 +4378,25 @@
         <v>205</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>209</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4410,25 +4410,25 @@
         <v>205</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>212</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4442,25 +4442,25 @@
         <v>205</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>215</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4474,121 +4474,121 @@
         <v>205</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>218</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>205</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>205</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>205</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4608,19 +4608,19 @@
         <v>247</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4640,19 +4640,19 @@
         <v>251</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4672,19 +4672,19 @@
         <v>255</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J80" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4704,19 +4704,19 @@
         <v>259</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4736,19 +4736,19 @@
         <v>263</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4768,19 +4768,19 @@
         <v>267</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4800,19 +4800,19 @@
         <v>271</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4832,51 +4832,51 @@
         <v>275</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>245</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4896,19 +4896,19 @@
         <v>279</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4928,19 +4928,19 @@
         <v>283</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4960,19 +4960,19 @@
         <v>287</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -4992,19 +4992,19 @@
         <v>291</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5024,19 +5024,19 @@
         <v>295</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5056,19 +5056,19 @@
         <v>299</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5088,19 +5088,19 @@
         <v>303</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5120,19 +5120,19 @@
         <v>307</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5152,19 +5152,19 @@
         <v>311</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5184,19 +5184,19 @@
         <v>315</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5216,19 +5216,19 @@
         <v>319</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5248,19 +5248,19 @@
         <v>323</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5280,19 +5280,19 @@
         <v>327</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5312,19 +5312,19 @@
         <v>331</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5344,19 +5344,19 @@
         <v>335</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5376,19 +5376,19 @@
         <v>339</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J102" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5408,19 +5408,19 @@
         <v>343</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J103" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5440,19 +5440,19 @@
         <v>347</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5472,19 +5472,19 @@
         <v>351</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5504,24 +5504,24 @@
         <v>355</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>356</v>
@@ -5536,19 +5536,19 @@
         <v>358</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5568,19 +5568,19 @@
         <v>362</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5600,19 +5600,19 @@
         <v>366</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5632,19 +5632,19 @@
         <v>370</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J110" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5664,19 +5664,19 @@
         <v>374</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5696,19 +5696,19 @@
         <v>378</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5728,19 +5728,19 @@
         <v>382</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5760,19 +5760,19 @@
         <v>386</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J114" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5792,19 +5792,19 @@
         <v>387</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J115" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5824,19 +5824,19 @@
         <v>391</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5856,19 +5856,19 @@
         <v>395</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J117" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5888,19 +5888,19 @@
         <v>399</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5920,19 +5920,19 @@
         <v>403</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5952,19 +5952,19 @@
         <v>407</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -5984,19 +5984,19 @@
         <v>411</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J121" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -6016,19 +6016,19 @@
         <v>415</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -6048,115 +6048,115 @@
         <v>419</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="J123" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>245</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>245</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>245</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>